<commit_message>
Build is added for Jenkins
</commit_message>
<xml_diff>
--- a/src/main/resources/newExcel2.xlsx
+++ b/src/main/resources/newExcel2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="106">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -194,6 +194,150 @@
   </si>
   <si>
     <t>20201113_095303</t>
+  </si>
+  <si>
+    <t>testing-jdbc-country-functionality;country-tetsing-with-jdbc</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>20201116_204157</t>
+  </si>
+  <si>
+    <t>20201116_204355</t>
+  </si>
+  <si>
+    <t>20201116_204421</t>
+  </si>
+  <si>
+    <t>20201116_204544</t>
+  </si>
+  <si>
+    <t>20201116_210252</t>
+  </si>
+  <si>
+    <t>20201116_210352</t>
+  </si>
+  <si>
+    <t>20201116_210520</t>
+  </si>
+  <si>
+    <t>20201116_211551</t>
+  </si>
+  <si>
+    <t>20201116_211626</t>
+  </si>
+  <si>
+    <t>20201116_211702</t>
+  </si>
+  <si>
+    <t>20201116_211754</t>
+  </si>
+  <si>
+    <t>20201116_211954</t>
+  </si>
+  <si>
+    <t>20201116_212020</t>
+  </si>
+  <si>
+    <t>20201116_214112</t>
+  </si>
+  <si>
+    <t>20201116_220108</t>
+  </si>
+  <si>
+    <t>20201116_221813</t>
+  </si>
+  <si>
+    <t>20201116_221854</t>
+  </si>
+  <si>
+    <t>20201116_221931</t>
+  </si>
+  <si>
+    <t>20201116_222108</t>
+  </si>
+  <si>
+    <t>20201116_222350</t>
+  </si>
+  <si>
+    <t>20201118_220859</t>
+  </si>
+  <si>
+    <t>20201118_220952</t>
+  </si>
+  <si>
+    <t>20201118_222404</t>
+  </si>
+  <si>
+    <t>20201118_223525</t>
+  </si>
+  <si>
+    <t>20201118_223750</t>
+  </si>
+  <si>
+    <t>20201118_223909</t>
+  </si>
+  <si>
+    <t>20201118_224259</t>
+  </si>
+  <si>
+    <t>20201118_224839</t>
+  </si>
+  <si>
+    <t>testing-jdbc-city-functionality;city-tetsing-with-jdbc</t>
+  </si>
+  <si>
+    <t>20201118_224935</t>
+  </si>
+  <si>
+    <t>20201118_224956</t>
+  </si>
+  <si>
+    <t>20201118_225024</t>
+  </si>
+  <si>
+    <t>20201119_004141</t>
+  </si>
+  <si>
+    <t>20201119_004235</t>
+  </si>
+  <si>
+    <t>20201119_004610</t>
+  </si>
+  <si>
+    <t>20201119_004714</t>
+  </si>
+  <si>
+    <t>20201119_022749</t>
+  </si>
+  <si>
+    <t>20201119_023158</t>
+  </si>
+  <si>
+    <t>20201119_023224</t>
+  </si>
+  <si>
+    <t>20201119_023312</t>
+  </si>
+  <si>
+    <t>20201119_023621</t>
+  </si>
+  <si>
+    <t>20201119_023643</t>
+  </si>
+  <si>
+    <t>20201119_023724</t>
+  </si>
+  <si>
+    <t>20201119_023750</t>
+  </si>
+  <si>
+    <t>20201119_024223</t>
+  </si>
+  <si>
+    <t>20201222_194026</t>
   </si>
 </sst>
 </file>
@@ -290,7 +434,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
@@ -1019,6 +1163,771 @@
         <v>20</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>71</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" t="s">
+        <v>79</v>
+      </c>
+      <c r="E62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="s">
+        <v>85</v>
+      </c>
+      <c r="E68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" t="s">
+        <v>59</v>
+      </c>
+      <c r="D69" t="s">
+        <v>86</v>
+      </c>
+      <c r="E69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" t="s">
+        <v>90</v>
+      </c>
+      <c r="E72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" t="s">
+        <v>59</v>
+      </c>
+      <c r="D74" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C76" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" t="s">
+        <v>94</v>
+      </c>
+      <c r="E76" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" t="s">
+        <v>95</v>
+      </c>
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>88</v>
+      </c>
+      <c r="C78" t="s">
+        <v>59</v>
+      </c>
+      <c r="D78" t="s">
+        <v>96</v>
+      </c>
+      <c r="E78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" t="s">
+        <v>59</v>
+      </c>
+      <c r="D79" t="s">
+        <v>97</v>
+      </c>
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" t="s">
+        <v>59</v>
+      </c>
+      <c r="D80" t="s">
+        <v>98</v>
+      </c>
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" t="s">
+        <v>59</v>
+      </c>
+      <c r="D81" t="s">
+        <v>99</v>
+      </c>
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" t="s">
+        <v>59</v>
+      </c>
+      <c r="D82" t="s">
+        <v>100</v>
+      </c>
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>88</v>
+      </c>
+      <c r="C83" t="s">
+        <v>59</v>
+      </c>
+      <c r="D83" t="s">
+        <v>101</v>
+      </c>
+      <c r="E83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" t="s">
+        <v>102</v>
+      </c>
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D85" t="s">
+        <v>103</v>
+      </c>
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86" t="s">
+        <v>59</v>
+      </c>
+      <c r="D86" t="s">
+        <v>104</v>
+      </c>
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>52</v>
+      </c>
+      <c r="C87" t="s">
+        <v>59</v>
+      </c>
+      <c r="D87" t="s">
+        <v>105</v>
+      </c>
+      <c r="E87" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
WindowSize is added to DriverClass
</commit_message>
<xml_diff>
--- a/src/main/resources/newExcel2.xlsx
+++ b/src/main/resources/newExcel2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="121">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -362,6 +362,27 @@
   </si>
   <si>
     <t>20201225_070040</t>
+  </si>
+  <si>
+    <t>20201225_224205</t>
+  </si>
+  <si>
+    <t>country-create-edit-delete-functionality;create-a-country</t>
+  </si>
+  <si>
+    <t>20201225_224222</t>
+  </si>
+  <si>
+    <t>country-create-edit-delete-functionality;edit-a-country</t>
+  </si>
+  <si>
+    <t>20201225_224249</t>
+  </si>
+  <si>
+    <t>country-create-edit-delete-functionality;delete-a-country</t>
+  </si>
+  <si>
+    <t>20201225_224316</t>
   </si>
 </sst>
 </file>
@@ -458,7 +479,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
@@ -2054,6 +2075,74 @@
         <v>20</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>52</v>
+      </c>
+      <c r="C94" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" t="s">
+        <v>114</v>
+      </c>
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>115</v>
+      </c>
+      <c r="C95" t="s">
+        <v>18</v>
+      </c>
+      <c r="D95" t="s">
+        <v>116</v>
+      </c>
+      <c r="E95" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>117</v>
+      </c>
+      <c r="C96" t="s">
+        <v>59</v>
+      </c>
+      <c r="D96" t="s">
+        <v>118</v>
+      </c>
+      <c r="E96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>119</v>
+      </c>
+      <c r="C97" t="s">
+        <v>59</v>
+      </c>
+      <c r="D97" t="s">
+        <v>120</v>
+      </c>
+      <c r="E97" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>